<commit_message>
update and fixing ,PRODUCT,RECIPE
fix UI
</commit_message>
<xml_diff>
--- a/PepperLunch/bin/Debug/Templates/Export.xlsx
+++ b/PepperLunch/bin/Debug/Templates/Export.xlsx
@@ -6,7 +6,7 @@
     <sheet name="Exported from Data Grid" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'Exported from Data Grid'!$A$1:$K$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'Exported from Data Grid'!$A$1:$M$7</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -38,6 +38,12 @@
     <t>POINT</t>
   </si>
   <si>
+    <t>STATE_RECEIPT</t>
+  </si>
+  <si>
+    <t>ADDRESS_RECEIPT</t>
+  </si>
+  <si>
     <t>CUSTOMER</t>
   </si>
   <si>
@@ -47,34 +53,68 @@
     <t>VOUCHER</t>
   </si>
   <si>
-    <t>ID001</t>
-  </si>
-  <si>
-    <t>ABCXYZ</t>
-  </si>
-  <si>
-    <t>KH01</t>
-  </si>
-  <si>
-    <t>PT1</t>
-  </si>
-  <si>
-    <t>DTO_PPL.CUSTOMER</t>
-  </si>
-  <si>
-    <t>DTO_PPL.METHOD_PAY</t>
-  </si>
-  <si>
-    <t>DTO_PPL.VOUCHER</t>
-  </si>
-  <si>
-    <t>ID002</t>
-  </si>
-  <si>
-    <t>ID003</t>
-  </si>
-  <si>
-    <t>ID004</t>
+    <t>-N3hpyZfsUOy3VzTgTMB</t>
+  </si>
+  <si>
+    <t>-N3Mz27GMSqHrwI-nA72</t>
+  </si>
+  <si>
+    <t>METHOD03</t>
+  </si>
+  <si>
+    <t>le trong tan</t>
+  </si>
+  <si>
+    <t>-N3qt_s-tRzVAcPyltsg</t>
+  </si>
+  <si>
+    <t>VOUCHER202261233914761</t>
+  </si>
+  <si>
+    <t>hcm</t>
+  </si>
+  <si>
+    <t>-N3VJNLG55xPxkjyXcoW</t>
+  </si>
+  <si>
+    <t>VOUCHER202261233859776</t>
+  </si>
+  <si>
+    <t>-N3SI0S_mS-c3y1oQZ2w</t>
+  </si>
+  <si>
+    <t>METHOD02</t>
+  </si>
+  <si>
+    <t>le Trong tan</t>
+  </si>
+  <si>
+    <t>-N3Wqfs8cUPrIah6QeWz</t>
+  </si>
+  <si>
+    <t>-N3VFm4yrByvz9ZnbRcd</t>
+  </si>
+  <si>
+    <t>sài gòn nè</t>
+  </si>
+  <si>
+    <t>-N3Wxbaw5YXcvcAjv9vx</t>
+  </si>
+  <si>
+    <t>VOUCHER202261233849144</t>
+  </si>
+  <si>
+    <t>-N3WvuOPScKmaNv8eeM4</t>
+  </si>
+  <si>
+    <t>sài gòn</t>
+  </si>
+  <si>
+    <t>-N3WyHrYfXen3eCWqPlE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hcm
+</t>
   </si>
 </sst>
 </file>
@@ -409,17 +449,19 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="16.44" customWidth="1" style="1"/>
-    <col min="2" max="2" width="16.44" customWidth="1" style="1"/>
-    <col min="3" max="3" width="16.44" customWidth="1" style="1"/>
-    <col min="4" max="4" width="16.44" customWidth="1" style="1"/>
-    <col min="5" max="5" width="16.44" customWidth="1" style="2"/>
-    <col min="6" max="6" width="16.44" customWidth="1" style="1"/>
-    <col min="7" max="7" width="16.44" customWidth="1" style="1"/>
-    <col min="8" max="8" width="16.44" customWidth="1" style="1"/>
-    <col min="9" max="9" width="16.44" customWidth="1" style="1"/>
-    <col min="10" max="10" width="16.44" customWidth="1" style="1"/>
-    <col min="11" max="11" width="16.67" customWidth="1" style="1"/>
+    <col min="1" max="1" width="13.78" customWidth="1" style="1"/>
+    <col min="2" max="2" width="13.78" customWidth="1" style="1"/>
+    <col min="3" max="3" width="13.78" customWidth="1" style="1"/>
+    <col min="4" max="4" width="13.78" customWidth="1" style="1"/>
+    <col min="5" max="5" width="13.78" customWidth="1" style="2"/>
+    <col min="6" max="6" width="13.78" customWidth="1" style="1"/>
+    <col min="7" max="7" width="13.78" customWidth="1" style="1"/>
+    <col min="8" max="8" width="13.78" customWidth="1" style="1"/>
+    <col min="9" max="9" width="13.78" customWidth="1" style="1"/>
+    <col min="10" max="10" width="13.78" customWidth="1" style="1"/>
+    <col min="11" max="11" width="13.78" customWidth="1" style="1"/>
+    <col min="12" max="12" width="13.78" customWidth="1" style="1"/>
+    <col min="13" max="13" width="15.11" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,140 +498,204 @@
       <c t="s" r="K1" s="1">
         <v>10</v>
       </c>
+      <c t="s" r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c t="s" r="M1" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" r="A2" s="1">
-        <v>11</v>
-      </c>
-      <c t="s" r="B2" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c t="s" r="C2" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c t="s" r="D2" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
-        <v>40179</v>
+        <v>44722.887428305061</v>
       </c>
       <c r="F2" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>5000000</v>
+        <v>369000</v>
       </c>
       <c r="H2" s="1">
-        <v>10</v>
-      </c>
-      <c t="s" r="I2" s="1">
-        <v>15</v>
+        <v>369000</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
       </c>
       <c t="s" r="J2" s="1">
         <v>16</v>
-      </c>
-      <c t="s" r="K2" s="1">
-        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3" s="1">
+        <v>17</v>
+      </c>
+      <c t="s" r="B3" s="1">
         <v>18</v>
       </c>
-      <c t="s" r="B3" s="1">
-        <v>12</v>
-      </c>
       <c t="s" r="C3" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c t="s" r="D3" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2">
-        <v>40179</v>
+        <v>44722.887428316702</v>
       </c>
       <c r="F3" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>5000000</v>
+        <v>299000</v>
       </c>
       <c r="H3" s="1">
-        <v>10</v>
-      </c>
-      <c t="s" r="I3" s="1">
-        <v>15</v>
+        <v>299000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
       </c>
       <c t="s" r="J3" s="1">
-        <v>16</v>
-      </c>
-      <c t="s" r="K3" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c t="s" r="A4" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c t="s" r="B4" s="1">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c t="s" r="C4" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c t="s" r="D4" s="1">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2">
-        <v>40179</v>
+        <v>44722.887428316702</v>
       </c>
       <c r="F4" s="1">
-        <v>130</v>
+        <v>3</v>
       </c>
       <c r="G4" s="1">
-        <v>5000000</v>
+        <v>977000</v>
       </c>
       <c r="H4" s="1">
-        <v>10</v>
-      </c>
-      <c t="s" r="I4" s="1">
-        <v>15</v>
+        <v>977000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
       </c>
       <c t="s" r="J4" s="1">
-        <v>16</v>
-      </c>
-      <c t="s" r="K4" s="1">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5" s="1">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c t="s" r="B5" s="1">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c t="s" r="C5" s="1">
+        <v>26</v>
+      </c>
+      <c t="s" r="D5" s="1">
+        <v>15</v>
       </c>
       <c r="E5" s="2">
-        <v>40179</v>
+        <v>44722.887428316702</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
-        <v>5000000</v>
+        <v>977000</v>
       </c>
       <c r="H5" s="1">
-        <v>10</v>
-      </c>
-      <c t="s" r="K5" s="1">
-        <v>17</v>
+        <v>977000</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c t="s" r="J5" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" r="A6" s="1">
+        <v>28</v>
+      </c>
+      <c t="s" r="B6" s="1">
+        <v>29</v>
+      </c>
+      <c t="s" r="C6" s="1">
+        <v>30</v>
+      </c>
+      <c t="s" r="D6" s="1">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44722.887428316702</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>369000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>369000</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+      <c t="s" r="J6" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" r="A7" s="1">
+        <v>32</v>
+      </c>
+      <c t="s" r="C7" s="1">
+        <v>30</v>
+      </c>
+      <c t="s" r="D7" s="1">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44722.887428316702</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>139000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>139000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c t="s" r="J7" s="1">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K5"/>
+  <autoFilter ref="A1:M7"/>
   <pageSetup fitToWidth="0" fitToHeight="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K5" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:M7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>